<commit_message>
modify models with exponential growth so they're suitable for verifying both discrete event and continuous integration: in one_rxn_exponential.xlsx, increase the species populations by 100x, modify their masses accordingly, & decrease the checkpoint period, & update the expected trajectories to reflect these changes; in one_exchange_rxn_compt_growth, improve accuracy of accounted_fraction_c in expected_predictions.py, decrease the reaction granularity by 10x, modify the rate law accordingly, & decrease the checkpoint period, & update the expected trajectories to reflect these changes; also loosen the absolute tolerance on ODE solutions; these changes increase the computing time for the verification tests
</commit_message>
<xml_diff>
--- a/tests/fixtures/dynamic_tests/one_rxn_exponential.xlsx
+++ b/tests/fixtures/dynamic_tests/one_rxn_exponential.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-21440" yWindow="7800" windowWidth="21080" windowHeight="13660" tabRatio="500" firstSheet="9" activeTab="9"/>
-    <workbookView xWindow="0" yWindow="6060" windowWidth="29240" windowHeight="15540" tabRatio="500" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="-21580" yWindow="10340" windowWidth="21080" windowHeight="11260" tabRatio="500" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="6060" windowWidth="34360" windowHeight="15540" tabRatio="500" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -796,9 +796,6 @@
     <t>Computation for Pop_B_c_</t>
   </si>
   <si>
-    <t>Computation for pop B in expected_exponential_pops.py</t>
-  </si>
-  <si>
     <t>Mass is constant because there are no exchange reactions and the 1 reaction is mass balanced</t>
   </si>
   <si>
@@ -806,6 +803,9 @@
   </si>
   <si>
     <t>Similarly, accounted mass is constant</t>
+  </si>
+  <si>
+    <t>Computation for pop B in expected_predictions.py</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1008,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1126,9 +1126,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1808,22 +1805,20 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="A3" sqref="A3:A8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125"/>
     <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125"/>
     <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1843,7 +1838,7 @@
       <c r="K1" s="36"/>
       <c r="L1" s="36"/>
     </row>
-    <row r="2" spans="1:12" s="53" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="52" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>200</v>
       </c>
@@ -1868,110 +1863,470 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>900</v>
+        <v>90000</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D8" si="0">init_pop_A - (E3 - init_pop_B)</f>
-        <v>900</v>
+        <f>init_pop_A - (E3 - init_pop_B)</f>
+        <v>90000</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="F3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>851</v>
+        <v>89167</v>
       </c>
       <c r="C4">
-        <v>149</v>
+        <v>10833</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>851</v>
+        <f>init_pop_A - (E4 - init_pop_B)</f>
+        <v>89167</v>
       </c>
       <c r="E4">
-        <v>149</v>
+        <v>10833</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>777</v>
+        <v>88265</v>
       </c>
       <c r="C5">
-        <v>223</v>
+        <v>11735</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>777</v>
+        <f>init_pop_A - (E5 - init_pop_B)</f>
+        <v>88265</v>
       </c>
       <c r="E5">
-        <v>223</v>
+        <v>11735</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>668</v>
+        <v>87288</v>
       </c>
       <c r="C6">
-        <v>332</v>
+        <v>12712</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>668</v>
+        <f>init_pop_A - (E6 - init_pop_B)</f>
+        <v>87288</v>
       </c>
       <c r="E6">
-        <v>332</v>
+        <v>12712</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>505</v>
+        <v>86229</v>
       </c>
       <c r="C7">
-        <v>495</v>
+        <v>13771</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>505</v>
+        <f>init_pop_A - (E7 - init_pop_B)</f>
+        <v>86229</v>
       </c>
       <c r="E7">
-        <v>495</v>
+        <v>13771</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>85082</v>
+      </c>
+      <c r="C8">
+        <v>14918</v>
+      </c>
+      <c r="D8">
+        <f>init_pop_A - (E8 - init_pop_B)</f>
+        <v>85082</v>
+      </c>
+      <c r="E8">
+        <v>14918</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>83839</v>
+      </c>
+      <c r="C9">
+        <v>16161</v>
+      </c>
+      <c r="D9">
+        <f>init_pop_A - (E9 - init_pop_B)</f>
+        <v>83839</v>
+      </c>
+      <c r="E9">
+        <v>16161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>82493</v>
+      </c>
+      <c r="C10">
+        <v>17507</v>
+      </c>
+      <c r="D10">
+        <f>init_pop_A - (E10 - init_pop_B)</f>
+        <v>82493</v>
+      </c>
+      <c r="E10">
+        <v>17507</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>81035</v>
+      </c>
+      <c r="C11">
+        <v>18965</v>
+      </c>
+      <c r="D11">
+        <f>init_pop_A - (E11 - init_pop_B)</f>
+        <v>81035</v>
+      </c>
+      <c r="E11">
+        <v>18965</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>79456</v>
+      </c>
+      <c r="C12">
+        <v>20544</v>
+      </c>
+      <c r="D12">
+        <f>init_pop_A - (E12 - init_pop_B)</f>
+        <v>79456</v>
+      </c>
+      <c r="E12">
+        <v>20544</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>77745</v>
+      </c>
+      <c r="C13">
+        <v>22255</v>
+      </c>
+      <c r="D13">
+        <f>init_pop_A - (E13 - init_pop_B)</f>
+        <v>77745</v>
+      </c>
+      <c r="E13">
+        <v>22255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>75891</v>
+      </c>
+      <c r="C14">
+        <v>24109</v>
+      </c>
+      <c r="D14">
+        <f>init_pop_A - (E14 - init_pop_B)</f>
+        <v>75891</v>
+      </c>
+      <c r="E14">
+        <v>24109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>73883</v>
+      </c>
+      <c r="C15">
+        <v>26117</v>
+      </c>
+      <c r="D15">
+        <f>init_pop_A - (E15 - init_pop_B)</f>
+        <v>73883</v>
+      </c>
+      <c r="E15">
+        <v>26117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>71708</v>
+      </c>
+      <c r="C16">
+        <v>28292</v>
+      </c>
+      <c r="D16">
+        <f>init_pop_A - (E16 - init_pop_B)</f>
+        <v>71708</v>
+      </c>
+      <c r="E16">
+        <v>28292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>69351</v>
+      </c>
+      <c r="C17">
+        <v>30649</v>
+      </c>
+      <c r="D17">
+        <f>init_pop_A - (E17 - init_pop_B)</f>
+        <v>69351</v>
+      </c>
+      <c r="E17">
+        <v>30649</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>66799</v>
+      </c>
+      <c r="C18">
+        <v>33201</v>
+      </c>
+      <c r="D18">
+        <f>init_pop_A - (E18 - init_pop_B)</f>
+        <v>66799</v>
+      </c>
+      <c r="E18">
+        <v>33201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>64034</v>
+      </c>
+      <c r="C19">
+        <v>35966</v>
+      </c>
+      <c r="D19">
+        <f>init_pop_A - (E19 - init_pop_B)</f>
+        <v>64034</v>
+      </c>
+      <c r="E19">
+        <v>35966</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>34</v>
+      </c>
+      <c r="B20">
+        <v>61038</v>
+      </c>
+      <c r="C20">
+        <v>38962</v>
+      </c>
+      <c r="D20">
+        <f>init_pop_A - (E20 - init_pop_B)</f>
+        <v>61038</v>
+      </c>
+      <c r="E20">
+        <v>38962</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>36</v>
+      </c>
+      <c r="B21">
+        <v>57793</v>
+      </c>
+      <c r="C21">
+        <v>42207</v>
+      </c>
+      <c r="D21">
+        <f>init_pop_A - (E21 - init_pop_B)</f>
+        <v>57793</v>
+      </c>
+      <c r="E21">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>54278</v>
+      </c>
+      <c r="C22">
+        <v>45722</v>
+      </c>
+      <c r="D22">
+        <f>init_pop_A - (E22 - init_pop_B)</f>
+        <v>54278</v>
+      </c>
+      <c r="E22">
+        <v>45722</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>40</v>
+      </c>
+      <c r="B23">
+        <v>50470</v>
+      </c>
+      <c r="C23">
+        <v>49530</v>
+      </c>
+      <c r="D23">
+        <f>init_pop_A - (E23 - init_pop_B)</f>
+        <v>50470</v>
+      </c>
+      <c r="E23">
+        <v>49530</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>42</v>
+      </c>
+      <c r="B24">
+        <v>46344</v>
+      </c>
+      <c r="C24">
+        <v>53656</v>
+      </c>
+      <c r="D24">
+        <f>init_pop_A - (E24 - init_pop_B)</f>
+        <v>46344</v>
+      </c>
+      <c r="E24">
+        <v>53656</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>44</v>
+      </c>
+      <c r="B25">
+        <v>41876</v>
+      </c>
+      <c r="C25">
+        <v>58124</v>
+      </c>
+      <c r="D25">
+        <f>init_pop_A - (E25 - init_pop_B)</f>
+        <v>41876</v>
+      </c>
+      <c r="E25">
+        <v>58124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>46</v>
+      </c>
+      <c r="B26">
+        <v>37035</v>
+      </c>
+      <c r="C26">
+        <v>62965</v>
+      </c>
+      <c r="D26">
+        <f>init_pop_A - (E26 - init_pop_B)</f>
+        <v>37035</v>
+      </c>
+      <c r="E26">
+        <v>62965</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>31790</v>
+      </c>
+      <c r="C27">
+        <v>68210</v>
+      </c>
+      <c r="D27">
+        <f>init_pop_A - (E27 - init_pop_B)</f>
+        <v>31790</v>
+      </c>
+      <c r="E27">
+        <v>68210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
         <v>50</v>
       </c>
-      <c r="B8">
-        <v>261</v>
-      </c>
-      <c r="C8">
-        <v>739</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>261</v>
-      </c>
-      <c r="E8">
-        <v>739</v>
+      <c r="B28">
+        <v>26109</v>
+      </c>
+      <c r="C28">
+        <v>73891</v>
+      </c>
+      <c r="D28">
+        <f>init_pop_A - (E28 - init_pop_B)</f>
+        <v>26109</v>
+      </c>
+      <c r="E28">
+        <v>73891</v>
       </c>
     </row>
   </sheetData>
@@ -1982,13 +2337,13 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
-      <selection activeCell="M3" sqref="M3:M8"/>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+      <selection activeCell="J3" sqref="J3:M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2012,59 +2367,59 @@
       <c r="K1" s="40"/>
       <c r="L1" s="40"/>
     </row>
-    <row r="2" spans="1:18" s="43" customFormat="1" ht="65" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:18" s="42" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="41" t="s">
         <v>201</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="41" t="s">
         <v>202</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="41" t="s">
         <v>204</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="41" t="s">
         <v>223</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="K2" s="42" t="s">
+      <c r="K2" s="41" t="s">
         <v>206</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="M2" s="42" t="s">
+      <c r="M2" s="41" t="s">
         <v>208</v>
       </c>
-      <c r="N2" s="42" t="s">
+      <c r="N2" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="O2" s="42" t="s">
+      <c r="O2" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="P2" s="42" t="s">
+      <c r="P2" s="41" t="s">
         <v>227</v>
       </c>
-      <c r="Q2" s="42" t="s">
+      <c r="Q2" s="41" t="s">
         <v>228</v>
       </c>
-      <c r="R2" s="42" t="s">
+      <c r="R2" s="41" t="s">
         <v>220</v>
       </c>
     </row>
@@ -2079,34 +2434,34 @@
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="L3">
-        <v>4.9816171212814925E-19</v>
+        <v>8.3026952021358202E-19</v>
       </c>
       <c r="M3">
-        <v>4.52874283752863E-22</v>
+        <v>7.5479047292143821E-22</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N8" si="0">density_c * volume_c</f>
+        <f t="shared" ref="N3:N28" si="0">density_c * volume_c</f>
         <v>1.0999999999999999E-18</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O8" si="1">volume_c</f>
+        <f t="shared" ref="O3:O28" si="1">volume_c</f>
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="P3">
         <f>(Molecular_weight_A *'!!Species trajectories'!D3 + Molecular_weight_B * '!!Species trajectories'!E3) / avogadros_constant</f>
-        <v>4.9816171212814925E-19</v>
+        <v>8.3026952021358202E-19</v>
       </c>
       <c r="Q3">
-        <f>P3/density_c</f>
-        <v>4.52874283752863E-22</v>
+        <f t="shared" ref="Q3:Q28" si="2">P3/density_c</f>
+        <v>7.5479047292143821E-22</v>
       </c>
       <c r="R3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J4">
         <v>1.0999999999999999E-18</v>
@@ -2115,10 +2470,10 @@
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="L4">
-        <v>4.9816171212814925E-19</v>
+        <v>8.3026952021358202E-19</v>
       </c>
       <c r="M4">
-        <v>4.52874283752863E-22</v>
+        <v>7.5479047292143821E-22</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
@@ -2130,19 +2485,19 @@
       </c>
       <c r="P4">
         <f>(Molecular_weight_A *'!!Species trajectories'!D4 + Molecular_weight_B * '!!Species trajectories'!E4) / avogadros_constant</f>
-        <v>4.9816171212814925E-19</v>
+        <v>8.3026952021358202E-19</v>
       </c>
       <c r="Q4">
-        <f>P4/density_c</f>
-        <v>4.52874283752863E-22</v>
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
       </c>
       <c r="R4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="J5">
         <v>1.0999999999999999E-18</v>
@@ -2151,10 +2506,10 @@
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="L5">
-        <v>4.9816171212814925E-19</v>
+        <v>8.3026952021358202E-19</v>
       </c>
       <c r="M5">
-        <v>4.52874283752863E-22</v>
+        <v>7.5479047292143821E-22</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
@@ -2166,19 +2521,19 @@
       </c>
       <c r="P5">
         <f>(Molecular_weight_A *'!!Species trajectories'!D5 + Molecular_weight_B * '!!Species trajectories'!E5) / avogadros_constant</f>
-        <v>4.9816171212814925E-19</v>
+        <v>8.3026952021358202E-19</v>
       </c>
       <c r="Q5">
-        <f>P5/density_c</f>
-        <v>4.52874283752863E-22</v>
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
       </c>
       <c r="R5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="J6">
         <v>1.0999999999999999E-18</v>
@@ -2187,10 +2542,10 @@
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="L6">
-        <v>4.9816171212814925E-19</v>
+        <v>8.3026952021358202E-19</v>
       </c>
       <c r="M6">
-        <v>4.52874283752863E-22</v>
+        <v>7.5479047292143821E-22</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
@@ -2202,16 +2557,16 @@
       </c>
       <c r="P6">
         <f>(Molecular_weight_A *'!!Species trajectories'!D6 + Molecular_weight_B * '!!Species trajectories'!E6) / avogadros_constant</f>
-        <v>4.9816171212814925E-19</v>
+        <v>8.3026952021358202E-19</v>
       </c>
       <c r="Q6">
-        <f>P6/density_c</f>
-        <v>4.52874283752863E-22</v>
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="J7">
         <v>1.0999999999999999E-18</v>
@@ -2220,10 +2575,10 @@
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="L7">
-        <v>4.9816171212814925E-19</v>
+        <v>8.3026952021358202E-19</v>
       </c>
       <c r="M7">
-        <v>4.52874283752863E-22</v>
+        <v>7.5479047292143821E-22</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
@@ -2235,16 +2590,16 @@
       </c>
       <c r="P7">
         <f>(Molecular_weight_A *'!!Species trajectories'!D7 + Molecular_weight_B * '!!Species trajectories'!E7) / avogadros_constant</f>
-        <v>4.9816171212814925E-19</v>
+        <v>8.3026952021358202E-19</v>
       </c>
       <c r="Q7">
-        <f>P7/density_c</f>
-        <v>4.52874283752863E-22</v>
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="J8">
         <v>1.0999999999999999E-18</v>
@@ -2253,10 +2608,10 @@
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="L8">
-        <v>4.9816171212814925E-19</v>
+        <v>8.3026952021358202E-19</v>
       </c>
       <c r="M8">
-        <v>4.52874283752863E-22</v>
+        <v>7.5479047292143821E-22</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
@@ -2268,15 +2623,672 @@
       </c>
       <c r="P8">
         <f>(Molecular_weight_A *'!!Species trajectories'!D8 + Molecular_weight_B * '!!Species trajectories'!E8) / avogadros_constant</f>
-        <v>4.9816171212814925E-19</v>
+        <v>8.3026952021358202E-19</v>
       </c>
       <c r="Q8">
-        <f>P8/density_c</f>
-        <v>4.52874283752863E-22</v>
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N9" s="41"/>
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K9">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L9">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M9">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P9">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D9 + Molecular_weight_B * '!!Species trajectories'!E9) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="J10">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K10">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L10">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M10">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P10">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D10 + Molecular_weight_B * '!!Species trajectories'!E10) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="J11">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K11">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L11">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M11">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P11">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D11 + Molecular_weight_B * '!!Species trajectories'!E11) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>18</v>
+      </c>
+      <c r="J12">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K12">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L12">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M12">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P12">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D12 + Molecular_weight_B * '!!Species trajectories'!E12) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="J13">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K13">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L13">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M13">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P13">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D13 + Molecular_weight_B * '!!Species trajectories'!E13) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>22</v>
+      </c>
+      <c r="J14">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K14">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L14">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M14">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P14">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D14 + Molecular_weight_B * '!!Species trajectories'!E14) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="J15">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K15">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L15">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M15">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P15">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D15 + Molecular_weight_B * '!!Species trajectories'!E15) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>26</v>
+      </c>
+      <c r="J16">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K16">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L16">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M16">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P16">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D16 + Molecular_weight_B * '!!Species trajectories'!E16) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>28</v>
+      </c>
+      <c r="J17">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K17">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L17">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M17">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P17">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D17 + Molecular_weight_B * '!!Species trajectories'!E17) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>30</v>
+      </c>
+      <c r="J18">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K18">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L18">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M18">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P18">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D18 + Molecular_weight_B * '!!Species trajectories'!E18) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>32</v>
+      </c>
+      <c r="J19">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K19">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L19">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M19">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P19">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D19 + Molecular_weight_B * '!!Species trajectories'!E19) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>34</v>
+      </c>
+      <c r="J20">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K20">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L20">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M20">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P20">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D20 + Molecular_weight_B * '!!Species trajectories'!E20) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>36</v>
+      </c>
+      <c r="J21">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K21">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L21">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M21">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P21">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D21 + Molecular_weight_B * '!!Species trajectories'!E21) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>38</v>
+      </c>
+      <c r="J22">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K22">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L22">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M22">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P22">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D22 + Molecular_weight_B * '!!Species trajectories'!E22) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>40</v>
+      </c>
+      <c r="J23">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K23">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L23">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M23">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P23">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D23 + Molecular_weight_B * '!!Species trajectories'!E23) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>42</v>
+      </c>
+      <c r="J24">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K24">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L24">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M24">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P24">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D24 + Molecular_weight_B * '!!Species trajectories'!E24) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>44</v>
+      </c>
+      <c r="J25">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K25">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L25">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M25">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P25">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D25 + Molecular_weight_B * '!!Species trajectories'!E25) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>46</v>
+      </c>
+      <c r="J26">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K26">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L26">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M26">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P26">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D26 + Molecular_weight_B * '!!Species trajectories'!E26) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>48</v>
+      </c>
+      <c r="J27">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K27">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L27">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M27">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P27">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D27 + Molecular_weight_B * '!!Species trajectories'!E27) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>50</v>
+      </c>
+      <c r="J28">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K28">
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="L28">
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="M28">
+        <v>7.5479047292143821E-22</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="P28">
+        <f>(Molecular_weight_A *'!!Species trajectories'!D28 + Molecular_weight_B * '!!Species trajectories'!E28) / avogadros_constant</f>
+        <v>8.3026952021358202E-19</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="2"/>
+        <v>7.5479047292143821E-22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2291,30 +3303,32 @@
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" s="43" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:5" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A1" s="50" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>217</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="50" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="50" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:5" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:5" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:5" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:5" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:5" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2495,11 +3509,11 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -3538,28 +4552,28 @@
       <c r="F3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="H3" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="M3" s="44" t="s">
+      <c r="M3" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="44" t="s">
+      <c r="N3" s="43" t="s">
         <v>51</v>
       </c>
       <c r="O3" s="6"/>
@@ -5029,7 +6043,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="C5" sqref="C5"/>
@@ -5037,7 +6051,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="16" customWidth="1"/>
     <col min="2" max="2" width="31.1640625" style="16" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" style="16" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="16" customWidth="1"/>
@@ -5045,7 +6059,7 @@
     <col min="6" max="6" width="16.83203125" style="16" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="16" customWidth="1"/>
     <col min="8" max="9" width="9.5" style="16" customWidth="1"/>
-    <col min="10" max="10" width="13.5" style="45" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="44" customWidth="1"/>
     <col min="11" max="1026" width="8.83203125" style="1" customWidth="1"/>
     <col min="1027" max="1028" width="9" style="1" customWidth="1"/>
     <col min="1029" max="16384" width="9" style="1"/>
@@ -5099,7 +6113,7 @@
       <c r="B3" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="49">
+      <c r="D3" s="48">
         <v>0.3</v>
       </c>
       <c r="F3" s="16" t="s">
@@ -5126,13 +6140,13 @@
       <c r="A5" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="50">
+      <c r="D5" s="49">
         <v>6.0221408570000002E+23</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="J5" s="46" t="s">
+      <c r="J5" s="45" t="s">
         <v>209</v>
       </c>
     </row>
@@ -5160,16 +6174,16 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="47" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
       <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5262,26 +6276,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="61" t="s">
+      <c r="G2" s="60" t="s">
         <v>141</v>
       </c>
-      <c r="H2" s="59"/>
-      <c r="I2" s="61" t="s">
+      <c r="H2" s="58"/>
+      <c r="I2" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="Q2" s="62" t="s">
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="Q2" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="R2" s="59"/>
-      <c r="S2" s="62" t="s">
+      <c r="R2" s="58"/>
+      <c r="S2" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="T2" s="59"/>
+      <c r="T2" s="58"/>
     </row>
     <row r="3" spans="1:23" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5449,10 +6463,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="61" t="s">
         <v>155</v>
       </c>
-      <c r="H2" s="59"/>
+      <c r="H2" s="58"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -6051,19 +7065,19 @@
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="56"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="55"/>
       <c r="L2" s="31"/>
-      <c r="M2" s="57" t="s">
+      <c r="M2" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -8222,7 +9236,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
       <selection activeCell="J8" sqref="J8"/>
@@ -8250,14 +9264,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -8315,7 +9329,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4">
-        <v>300</v>
+        <v>5</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -8337,7 +9351,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5">
-        <v>300</v>
+        <v>5</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -8461,8 +9475,8 @@
   <sheetPr codeName="Sheet9" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
       <selection activeCell="C3" sqref="A3:C4"/>
@@ -8544,7 +9558,7 @@
         <v>80</v>
       </c>
       <c r="E3">
-        <v>900</v>
+        <v>90000</v>
       </c>
       <c r="F3" s="27"/>
       <c r="G3" s="34" t="s">
@@ -8563,7 +9577,7 @@
         <v>80</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="F4" s="27"/>
       <c r="G4" s="34" t="s">

</xml_diff>

<commit_message>
measure performance of dynamic_tests and speed up one_rxn_exponential.xlsx
</commit_message>
<xml_diff>
--- a/tests/fixtures/dynamic_tests/one_rxn_exponential.xlsx
+++ b/tests/fixtures/dynamic_tests/one_rxn_exponential.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-21580" yWindow="10340" windowWidth="21080" windowHeight="11260" tabRatio="500" firstSheet="6" activeTab="8"/>
-    <workbookView xWindow="0" yWindow="6060" windowWidth="34360" windowHeight="15540" tabRatio="500" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="-21580" yWindow="10340" windowWidth="21080" windowHeight="11260" tabRatio="500" firstSheet="12" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="2660" windowWidth="34360" windowHeight="18940" tabRatio="500" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -1805,13 +1805,13 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="A14" sqref="A14:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1869,7 +1869,7 @@
         <v>10000</v>
       </c>
       <c r="D3">
-        <f>init_pop_A - (E3 - init_pop_B)</f>
+        <f t="shared" ref="D3:D13" si="0">init_pop_A - (E3 - init_pop_B)</f>
         <v>90000</v>
       </c>
       <c r="E3">
@@ -1890,7 +1890,7 @@
         <v>10833</v>
       </c>
       <c r="D4">
-        <f>init_pop_A - (E4 - init_pop_B)</f>
+        <f t="shared" si="0"/>
         <v>89167</v>
       </c>
       <c r="E4">
@@ -1908,7 +1908,7 @@
         <v>11735</v>
       </c>
       <c r="D5">
-        <f>init_pop_A - (E5 - init_pop_B)</f>
+        <f t="shared" si="0"/>
         <v>88265</v>
       </c>
       <c r="E5">
@@ -1926,7 +1926,7 @@
         <v>12712</v>
       </c>
       <c r="D6">
-        <f>init_pop_A - (E6 - init_pop_B)</f>
+        <f t="shared" si="0"/>
         <v>87288</v>
       </c>
       <c r="E6">
@@ -1944,7 +1944,7 @@
         <v>13771</v>
       </c>
       <c r="D7">
-        <f>init_pop_A - (E7 - init_pop_B)</f>
+        <f t="shared" si="0"/>
         <v>86229</v>
       </c>
       <c r="E7">
@@ -1962,7 +1962,7 @@
         <v>14918</v>
       </c>
       <c r="D8">
-        <f>init_pop_A - (E8 - init_pop_B)</f>
+        <f t="shared" si="0"/>
         <v>85082</v>
       </c>
       <c r="E8">
@@ -1980,7 +1980,7 @@
         <v>16161</v>
       </c>
       <c r="D9">
-        <f>init_pop_A - (E9 - init_pop_B)</f>
+        <f t="shared" si="0"/>
         <v>83839</v>
       </c>
       <c r="E9">
@@ -1998,7 +1998,7 @@
         <v>17507</v>
       </c>
       <c r="D10">
-        <f>init_pop_A - (E10 - init_pop_B)</f>
+        <f t="shared" si="0"/>
         <v>82493</v>
       </c>
       <c r="E10">
@@ -2016,7 +2016,7 @@
         <v>18965</v>
       </c>
       <c r="D11">
-        <f>init_pop_A - (E11 - init_pop_B)</f>
+        <f t="shared" si="0"/>
         <v>81035</v>
       </c>
       <c r="E11">
@@ -2034,7 +2034,7 @@
         <v>20544</v>
       </c>
       <c r="D12">
-        <f>init_pop_A - (E12 - init_pop_B)</f>
+        <f t="shared" si="0"/>
         <v>79456</v>
       </c>
       <c r="E12">
@@ -2052,281 +2052,11 @@
         <v>22255</v>
       </c>
       <c r="D13">
-        <f>init_pop_A - (E13 - init_pop_B)</f>
+        <f t="shared" si="0"/>
         <v>77745</v>
       </c>
       <c r="E13">
         <v>22255</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>22</v>
-      </c>
-      <c r="B14">
-        <v>75891</v>
-      </c>
-      <c r="C14">
-        <v>24109</v>
-      </c>
-      <c r="D14">
-        <f>init_pop_A - (E14 - init_pop_B)</f>
-        <v>75891</v>
-      </c>
-      <c r="E14">
-        <v>24109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>24</v>
-      </c>
-      <c r="B15">
-        <v>73883</v>
-      </c>
-      <c r="C15">
-        <v>26117</v>
-      </c>
-      <c r="D15">
-        <f>init_pop_A - (E15 - init_pop_B)</f>
-        <v>73883</v>
-      </c>
-      <c r="E15">
-        <v>26117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>26</v>
-      </c>
-      <c r="B16">
-        <v>71708</v>
-      </c>
-      <c r="C16">
-        <v>28292</v>
-      </c>
-      <c r="D16">
-        <f>init_pop_A - (E16 - init_pop_B)</f>
-        <v>71708</v>
-      </c>
-      <c r="E16">
-        <v>28292</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>28</v>
-      </c>
-      <c r="B17">
-        <v>69351</v>
-      </c>
-      <c r="C17">
-        <v>30649</v>
-      </c>
-      <c r="D17">
-        <f>init_pop_A - (E17 - init_pop_B)</f>
-        <v>69351</v>
-      </c>
-      <c r="E17">
-        <v>30649</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>30</v>
-      </c>
-      <c r="B18">
-        <v>66799</v>
-      </c>
-      <c r="C18">
-        <v>33201</v>
-      </c>
-      <c r="D18">
-        <f>init_pop_A - (E18 - init_pop_B)</f>
-        <v>66799</v>
-      </c>
-      <c r="E18">
-        <v>33201</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>32</v>
-      </c>
-      <c r="B19">
-        <v>64034</v>
-      </c>
-      <c r="C19">
-        <v>35966</v>
-      </c>
-      <c r="D19">
-        <f>init_pop_A - (E19 - init_pop_B)</f>
-        <v>64034</v>
-      </c>
-      <c r="E19">
-        <v>35966</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>34</v>
-      </c>
-      <c r="B20">
-        <v>61038</v>
-      </c>
-      <c r="C20">
-        <v>38962</v>
-      </c>
-      <c r="D20">
-        <f>init_pop_A - (E20 - init_pop_B)</f>
-        <v>61038</v>
-      </c>
-      <c r="E20">
-        <v>38962</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>36</v>
-      </c>
-      <c r="B21">
-        <v>57793</v>
-      </c>
-      <c r="C21">
-        <v>42207</v>
-      </c>
-      <c r="D21">
-        <f>init_pop_A - (E21 - init_pop_B)</f>
-        <v>57793</v>
-      </c>
-      <c r="E21">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>38</v>
-      </c>
-      <c r="B22">
-        <v>54278</v>
-      </c>
-      <c r="C22">
-        <v>45722</v>
-      </c>
-      <c r="D22">
-        <f>init_pop_A - (E22 - init_pop_B)</f>
-        <v>54278</v>
-      </c>
-      <c r="E22">
-        <v>45722</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>40</v>
-      </c>
-      <c r="B23">
-        <v>50470</v>
-      </c>
-      <c r="C23">
-        <v>49530</v>
-      </c>
-      <c r="D23">
-        <f>init_pop_A - (E23 - init_pop_B)</f>
-        <v>50470</v>
-      </c>
-      <c r="E23">
-        <v>49530</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>42</v>
-      </c>
-      <c r="B24">
-        <v>46344</v>
-      </c>
-      <c r="C24">
-        <v>53656</v>
-      </c>
-      <c r="D24">
-        <f>init_pop_A - (E24 - init_pop_B)</f>
-        <v>46344</v>
-      </c>
-      <c r="E24">
-        <v>53656</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>44</v>
-      </c>
-      <c r="B25">
-        <v>41876</v>
-      </c>
-      <c r="C25">
-        <v>58124</v>
-      </c>
-      <c r="D25">
-        <f>init_pop_A - (E25 - init_pop_B)</f>
-        <v>41876</v>
-      </c>
-      <c r="E25">
-        <v>58124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>46</v>
-      </c>
-      <c r="B26">
-        <v>37035</v>
-      </c>
-      <c r="C26">
-        <v>62965</v>
-      </c>
-      <c r="D26">
-        <f>init_pop_A - (E26 - init_pop_B)</f>
-        <v>37035</v>
-      </c>
-      <c r="E26">
-        <v>62965</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>48</v>
-      </c>
-      <c r="B27">
-        <v>31790</v>
-      </c>
-      <c r="C27">
-        <v>68210</v>
-      </c>
-      <c r="D27">
-        <f>init_pop_A - (E27 - init_pop_B)</f>
-        <v>31790</v>
-      </c>
-      <c r="E27">
-        <v>68210</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>50</v>
-      </c>
-      <c r="B28">
-        <v>26109</v>
-      </c>
-      <c r="C28">
-        <v>73891</v>
-      </c>
-      <c r="D28">
-        <f>init_pop_A - (E28 - init_pop_B)</f>
-        <v>26109</v>
-      </c>
-      <c r="E28">
-        <v>73891</v>
       </c>
     </row>
   </sheetData>
@@ -2337,13 +2067,13 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
-    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
-      <selection activeCell="J3" sqref="J3:M28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2440,11 +2170,11 @@
         <v>7.5479047292143821E-22</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N28" si="0">density_c * volume_c</f>
+        <f t="shared" ref="N3:N13" si="0">density_c * volume_c</f>
         <v>1.0999999999999999E-18</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O28" si="1">volume_c</f>
+        <f t="shared" ref="O3:O13" si="1">volume_c</f>
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="P3">
@@ -2452,7 +2182,7 @@
         <v>8.3026952021358202E-19</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q28" si="2">P3/density_c</f>
+        <f t="shared" ref="Q3:Q13" si="2">P3/density_c</f>
         <v>7.5479047292143821E-22</v>
       </c>
       <c r="R3" t="s">
@@ -2791,501 +2521,6 @@
         <v>8.3026952021358202E-19</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>22</v>
-      </c>
-      <c r="J14">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K14">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L14">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M14">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P14">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D14 + Molecular_weight_B * '!!Species trajectories'!E14) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>24</v>
-      </c>
-      <c r="J15">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K15">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L15">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M15">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P15">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D15 + Molecular_weight_B * '!!Species trajectories'!E15) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>26</v>
-      </c>
-      <c r="J16">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K16">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L16">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M16">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P16">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D16 + Molecular_weight_B * '!!Species trajectories'!E16) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>28</v>
-      </c>
-      <c r="J17">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K17">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L17">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M17">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P17">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D17 + Molecular_weight_B * '!!Species trajectories'!E17) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>30</v>
-      </c>
-      <c r="J18">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K18">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L18">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M18">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P18">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D18 + Molecular_weight_B * '!!Species trajectories'!E18) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>32</v>
-      </c>
-      <c r="J19">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K19">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L19">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M19">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P19">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D19 + Molecular_weight_B * '!!Species trajectories'!E19) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>34</v>
-      </c>
-      <c r="J20">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K20">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L20">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M20">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P20">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D20 + Molecular_weight_B * '!!Species trajectories'!E20) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>36</v>
-      </c>
-      <c r="J21">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K21">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L21">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M21">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P21">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D21 + Molecular_weight_B * '!!Species trajectories'!E21) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>38</v>
-      </c>
-      <c r="J22">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K22">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L22">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M22">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P22">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D22 + Molecular_weight_B * '!!Species trajectories'!E22) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>40</v>
-      </c>
-      <c r="J23">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K23">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L23">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M23">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O23">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P23">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D23 + Molecular_weight_B * '!!Species trajectories'!E23) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>42</v>
-      </c>
-      <c r="J24">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K24">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L24">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M24">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P24">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D24 + Molecular_weight_B * '!!Species trajectories'!E24) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>44</v>
-      </c>
-      <c r="J25">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K25">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L25">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M25">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N25">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O25">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P25">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D25 + Molecular_weight_B * '!!Species trajectories'!E25) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>46</v>
-      </c>
-      <c r="J26">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K26">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L26">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M26">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N26">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O26">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P26">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D26 + Molecular_weight_B * '!!Species trajectories'!E26) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>48</v>
-      </c>
-      <c r="J27">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K27">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L27">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M27">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P27">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D27 + Molecular_weight_B * '!!Species trajectories'!E27) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="2"/>
-        <v>7.5479047292143821E-22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>50</v>
-      </c>
-      <c r="J28">
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="K28">
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="L28">
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="M28">
-        <v>7.5479047292143821E-22</v>
-      </c>
-      <c r="N28">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999E-18</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999991E-22</v>
-      </c>
-      <c r="P28">
-        <f>(Molecular_weight_A *'!!Species trajectories'!D28 + Molecular_weight_B * '!!Species trajectories'!E28) / avogadros_constant</f>
-        <v>8.3026952021358202E-19</v>
-      </c>
-      <c r="Q28">
         <f t="shared" si="2"/>
         <v>7.5479047292143821E-22</v>
       </c>
@@ -6041,9 +5276,9 @@
   <sheetPr codeName="Sheet20" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="C5" sqref="C5"/>
@@ -6167,7 +5402,7 @@
         <v>211</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>41</v>
@@ -9475,7 +8710,7 @@
   <sheetPr codeName="Sheet9" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">

</xml_diff>